<commit_message>
JPY STD without ON and TN
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/JPY_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/JPY_YCSTDBootstrapping.xlsx
@@ -1738,6 +1738,15 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="6" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1752,15 +1761,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="6" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2643,8 +2643,8 @@
         <v>68</v>
       </c>
       <c r="D14" s="22" t="e">
-        <f ca="1">qlPiecewiseYieldCurve(D16,NDays,Calendar,ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
+        <v>#NUM!</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -2686,9 +2686,9 @@
       <c r="C15" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="21" t="e">
+      <c r="D15" s="21" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(YieldCurve)</f>
-        <v>#NAME?</v>
+        <v>qlPiecewiseYieldCurve - operToVectorImpl: error converting parameter 'RateHelpers' to type 'class std::basic_string&lt;char,struct std::char_traits&lt;char&gt;,class std::allocator&lt;char&gt; &gt;' : Unable to convert type 'struct ObjectHandler::empty_property_tag' to typ</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>122</v>
@@ -2997,12 +2997,12 @@
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="9" t="e">
-        <f ca="1">_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D23" s="8" t="e">
-        <f ca="1">MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>#NAME?</v>
+        <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -3037,13 +3037,13 @@
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="7">
+      <c r="C24" s="7" t="e">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>52908</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D24" s="6" t="e">
-        <f ca="1">MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>#NAME?</v>
+        <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -3081,9 +3081,9 @@
       <c r="C25" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="71" t="e">
+      <c r="D25" s="71" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(Selected!J1)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -3123,8 +3123,8 @@
         <v>JPYSTD#0000</v>
       </c>
       <c r="D26" s="6" t="e">
-        <f ca="1">_xll.qlRelinkableHandleLinkTo(C26,YieldCurve)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRelinkableHandleLinkTo(C26,YieldCurve)</f>
+        <v>#NUM!</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -3163,8 +3163,8 @@
         <v>123</v>
       </c>
       <c r="D27" s="44" t="e">
-        <f ca="1">_xll.qlExtrapolatorEnableExtrapolation(YieldCurve,TRUE)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlExtrapolatorEnableExtrapolation(YieldCurve,TRUE)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -4558,11 +4558,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="191" t="s">
+      <c r="B1" s="194" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="192"/>
-      <c r="D1" s="193"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="196"/>
       <c r="E1" s="114" t="s">
         <v>49</v>
       </c>
@@ -4611,7 +4611,6 @@
       </c>
       <c r="H2" s="118"/>
       <c r="I2" s="65" t="b">
-        <f>IF(ISERROR(G2),FALSE,TRUE)</f>
         <v>0</v>
       </c>
       <c r="J2" s="65">
@@ -4655,8 +4654,7 @@
       </c>
       <c r="H3" s="118"/>
       <c r="I3" s="65" t="b">
-        <f t="shared" ref="I3:I9" si="0">IF(ISERROR(G3),FALSE,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="65">
         <v>10</v>
@@ -4699,7 +4697,6 @@
       </c>
       <c r="H4" s="118"/>
       <c r="I4" s="65" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J4" s="65">
@@ -4743,7 +4740,6 @@
       </c>
       <c r="H5" s="118"/>
       <c r="I5" s="65" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J5" s="65">
@@ -4787,7 +4783,6 @@
       </c>
       <c r="H6" s="118"/>
       <c r="I6" s="65" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J6" s="65">
@@ -4825,7 +4820,6 @@
       </c>
       <c r="H7" s="118"/>
       <c r="I7" s="65" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J7" s="65">
@@ -4863,7 +4857,6 @@
       </c>
       <c r="H8" s="118"/>
       <c r="I8" s="65" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J8" s="65">
@@ -4901,7 +4894,6 @@
       </c>
       <c r="H9" s="118"/>
       <c r="I9" s="65" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J9" s="65">
@@ -4927,7 +4919,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="133" t="str">
-        <f t="shared" ref="D10:D20" si="1">(B10+Months)&amp;"F"</f>
+        <f t="shared" ref="D10:D20" si="0">(B10+Months)&amp;"F"</f>
         <v>4F</v>
       </c>
       <c r="E10" s="133" t="str">
@@ -4969,7 +4961,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5F</v>
       </c>
       <c r="E11" s="117" t="str">
@@ -5011,7 +5003,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6F</v>
       </c>
       <c r="E12" s="117" t="str">
@@ -5053,7 +5045,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7F</v>
       </c>
       <c r="E13" s="117" t="str">
@@ -5095,7 +5087,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8F</v>
       </c>
       <c r="E14" s="117" t="str">
@@ -5137,7 +5129,7 @@
         <v>37</v>
       </c>
       <c r="D15" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9F</v>
       </c>
       <c r="E15" s="117" t="str">
@@ -5179,7 +5171,7 @@
         <v>37</v>
       </c>
       <c r="D16" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10F</v>
       </c>
       <c r="E16" s="117" t="str">
@@ -5221,7 +5213,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11F</v>
       </c>
       <c r="E17" s="117" t="str">
@@ -5263,7 +5255,7 @@
         <v>37</v>
       </c>
       <c r="D18" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12F</v>
       </c>
       <c r="E18" s="117" t="str">
@@ -5305,7 +5297,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13F</v>
       </c>
       <c r="E19" s="117" t="str">
@@ -5347,7 +5339,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14F</v>
       </c>
       <c r="E20" s="122" t="str">
@@ -5387,7 +5379,7 @@
       </c>
       <c r="B21" s="127"/>
       <c r="C21" s="116" t="str">
-        <f t="shared" ref="C21:C62" si="2">"FUT"&amp;IndexTenor</f>
+        <f t="shared" ref="C21:C62" si="1">"FUT"&amp;IndexTenor</f>
         <v>FUT3M</v>
       </c>
       <c r="D21" s="117" t="str">
@@ -5434,7 +5426,7 @@
       </c>
       <c r="B22" s="127"/>
       <c r="C22" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D22" s="117" t="str">
@@ -5480,7 +5472,7 @@
       </c>
       <c r="B23" s="127"/>
       <c r="C23" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D23" s="117" t="str">
@@ -5526,7 +5518,7 @@
       </c>
       <c r="B24" s="127"/>
       <c r="C24" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D24" s="117" t="str">
@@ -5572,7 +5564,7 @@
       </c>
       <c r="B25" s="127"/>
       <c r="C25" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D25" s="117" t="str">
@@ -5618,7 +5610,7 @@
       </c>
       <c r="B26" s="127"/>
       <c r="C26" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D26" s="117" t="str">
@@ -5664,7 +5656,7 @@
       </c>
       <c r="B27" s="127"/>
       <c r="C27" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D27" s="117" t="str">
@@ -5710,7 +5702,7 @@
       </c>
       <c r="B28" s="127"/>
       <c r="C28" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D28" s="117" t="str">
@@ -5756,7 +5748,7 @@
       </c>
       <c r="B29" s="127"/>
       <c r="C29" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D29" s="117" t="str">
@@ -5802,7 +5794,7 @@
       </c>
       <c r="B30" s="127"/>
       <c r="C30" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D30" s="117" t="str">
@@ -5848,7 +5840,7 @@
       </c>
       <c r="B31" s="127"/>
       <c r="C31" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D31" s="117" t="str">
@@ -5894,7 +5886,7 @@
       </c>
       <c r="B32" s="127"/>
       <c r="C32" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D32" s="117" t="str">
@@ -5940,7 +5932,7 @@
       </c>
       <c r="B33" s="127"/>
       <c r="C33" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D33" s="117" t="str">
@@ -5986,7 +5978,7 @@
       </c>
       <c r="B34" s="127"/>
       <c r="C34" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D34" s="117" t="str">
@@ -6032,7 +6024,7 @@
       </c>
       <c r="B35" s="127"/>
       <c r="C35" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D35" s="117" t="str">
@@ -6078,7 +6070,7 @@
       </c>
       <c r="B36" s="127"/>
       <c r="C36" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D36" s="117" t="str">
@@ -6124,7 +6116,7 @@
       </c>
       <c r="B37" s="127"/>
       <c r="C37" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D37" s="117" t="str">
@@ -6170,7 +6162,7 @@
       </c>
       <c r="B38" s="127"/>
       <c r="C38" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D38" s="117" t="str">
@@ -6216,7 +6208,7 @@
       </c>
       <c r="B39" s="127"/>
       <c r="C39" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D39" s="117" t="str">
@@ -6262,7 +6254,7 @@
       </c>
       <c r="B40" s="127"/>
       <c r="C40" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D40" s="117" t="str">
@@ -6308,7 +6300,7 @@
       </c>
       <c r="B41" s="127"/>
       <c r="C41" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D41" s="117" t="str">
@@ -6354,7 +6346,7 @@
       </c>
       <c r="B42" s="127"/>
       <c r="C42" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D42" s="117" t="str">
@@ -6400,7 +6392,7 @@
       </c>
       <c r="B43" s="127"/>
       <c r="C43" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D43" s="117" t="str">
@@ -6446,7 +6438,7 @@
       </c>
       <c r="B44" s="127"/>
       <c r="C44" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D44" s="117" t="str">
@@ -6492,7 +6484,7 @@
       </c>
       <c r="B45" s="127"/>
       <c r="C45" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D45" s="117" t="str">
@@ -6538,7 +6530,7 @@
       </c>
       <c r="B46" s="127"/>
       <c r="C46" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D46" s="117" t="str">
@@ -6584,7 +6576,7 @@
       </c>
       <c r="B47" s="127"/>
       <c r="C47" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D47" s="117" t="str">
@@ -6630,7 +6622,7 @@
       </c>
       <c r="B48" s="127"/>
       <c r="C48" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D48" s="117" t="str">
@@ -6676,7 +6668,7 @@
       </c>
       <c r="B49" s="127"/>
       <c r="C49" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D49" s="117" t="str">
@@ -6722,7 +6714,7 @@
       </c>
       <c r="B50" s="127"/>
       <c r="C50" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D50" s="117" t="str">
@@ -6768,7 +6760,7 @@
       </c>
       <c r="B51" s="127"/>
       <c r="C51" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D51" s="117" t="str">
@@ -6814,7 +6806,7 @@
       </c>
       <c r="B52" s="127"/>
       <c r="C52" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D52" s="117" t="str">
@@ -6861,7 +6853,7 @@
       </c>
       <c r="B53" s="127"/>
       <c r="C53" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D53" s="117" t="str">
@@ -6908,7 +6900,7 @@
       </c>
       <c r="B54" s="127"/>
       <c r="C54" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D54" s="117" t="str">
@@ -6955,7 +6947,7 @@
       </c>
       <c r="B55" s="127"/>
       <c r="C55" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D55" s="117" t="str">
@@ -7002,7 +6994,7 @@
       </c>
       <c r="B56" s="127"/>
       <c r="C56" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D56" s="117" t="str">
@@ -7049,7 +7041,7 @@
       </c>
       <c r="B57" s="127"/>
       <c r="C57" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D57" s="117" t="str">
@@ -7096,7 +7088,7 @@
       </c>
       <c r="B58" s="127"/>
       <c r="C58" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D58" s="117" t="str">
@@ -7143,7 +7135,7 @@
       </c>
       <c r="B59" s="127"/>
       <c r="C59" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D59" s="117" t="str">
@@ -7190,7 +7182,7 @@
       </c>
       <c r="B60" s="127"/>
       <c r="C60" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D60" s="117" t="str">
@@ -7237,7 +7229,7 @@
       </c>
       <c r="B61" s="127"/>
       <c r="C61" s="116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D61" s="117" t="str">
@@ -7284,7 +7276,7 @@
       </c>
       <c r="B62" s="128"/>
       <c r="C62" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>FUT3M</v>
       </c>
       <c r="D62" s="122" t="str">
@@ -7327,7 +7319,7 @@
     </row>
     <row r="63" spans="1:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="127">
-        <f t="shared" ref="B63:B94" si="3">SwapFixedFreq</f>
+        <f t="shared" ref="B63:B94" si="2">SwapFixedFreq</f>
         <v>0</v>
       </c>
       <c r="C63" s="116" t="s">
@@ -7373,7 +7365,7 @@
     </row>
     <row r="64" spans="1:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C64" s="116" t="s">
@@ -7419,7 +7411,7 @@
     </row>
     <row r="65" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C65" s="116" t="s">
@@ -7465,7 +7457,7 @@
     </row>
     <row r="66" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C66" s="116" t="s">
@@ -7511,7 +7503,7 @@
     </row>
     <row r="67" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C67" s="116" t="s">
@@ -7557,7 +7549,7 @@
     </row>
     <row r="68" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C68" s="116" t="s">
@@ -7603,7 +7595,7 @@
     </row>
     <row r="69" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C69" s="116" t="s">
@@ -7649,7 +7641,7 @@
     </row>
     <row r="70" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C70" s="116" t="s">
@@ -7695,7 +7687,7 @@
     </row>
     <row r="71" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C71" s="116" t="s">
@@ -7741,7 +7733,7 @@
     </row>
     <row r="72" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C72" s="116" t="s">
@@ -7787,7 +7779,7 @@
     </row>
     <row r="73" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C73" s="116" t="s">
@@ -7833,7 +7825,7 @@
     </row>
     <row r="74" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C74" s="116" t="s">
@@ -7879,7 +7871,7 @@
     </row>
     <row r="75" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C75" s="116" t="s">
@@ -7925,7 +7917,7 @@
     </row>
     <row r="76" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C76" s="116" t="s">
@@ -7971,7 +7963,7 @@
     </row>
     <row r="77" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C77" s="116" t="s">
@@ -8017,7 +8009,7 @@
     </row>
     <row r="78" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C78" s="116" t="s">
@@ -8063,7 +8055,7 @@
     </row>
     <row r="79" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C79" s="116" t="s">
@@ -8109,7 +8101,7 @@
     </row>
     <row r="80" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C80" s="116" t="s">
@@ -8155,7 +8147,7 @@
     </row>
     <row r="81" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C81" s="116" t="s">
@@ -8201,7 +8193,7 @@
     </row>
     <row r="82" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C82" s="116" t="s">
@@ -8247,7 +8239,7 @@
     </row>
     <row r="83" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C83" s="116" t="s">
@@ -8293,7 +8285,7 @@
     </row>
     <row r="84" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C84" s="116" t="s">
@@ -8339,7 +8331,7 @@
     </row>
     <row r="85" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C85" s="116" t="s">
@@ -8385,7 +8377,7 @@
     </row>
     <row r="86" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C86" s="116" t="s">
@@ -8431,7 +8423,7 @@
     </row>
     <row r="87" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C87" s="116" t="s">
@@ -8477,7 +8469,7 @@
     </row>
     <row r="88" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C88" s="116" t="s">
@@ -8523,7 +8515,7 @@
     </row>
     <row r="89" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C89" s="116" t="s">
@@ -8569,7 +8561,7 @@
     </row>
     <row r="90" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C90" s="116" t="s">
@@ -8614,7 +8606,7 @@
     </row>
     <row r="91" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C91" s="116" t="s">
@@ -8659,7 +8651,7 @@
     </row>
     <row r="92" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C92" s="116" t="s">
@@ -8704,7 +8696,7 @@
     </row>
     <row r="93" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C93" s="116" t="s">
@@ -8749,7 +8741,7 @@
     </row>
     <row r="94" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C94" s="116" t="s">
@@ -8794,7 +8786,7 @@
     </row>
     <row r="95" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="127">
-        <f t="shared" ref="B95:B99" si="4">SwapFixedFreq</f>
+        <f t="shared" ref="B95:B99" si="3">SwapFixedFreq</f>
         <v>0</v>
       </c>
       <c r="C95" s="116" t="s">
@@ -8839,7 +8831,7 @@
     </row>
     <row r="96" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C96" s="116" t="s">
@@ -8884,7 +8876,7 @@
     </row>
     <row r="97" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C97" s="116" t="s">
@@ -8929,7 +8921,7 @@
     </row>
     <row r="98" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C98" s="116" t="s">
@@ -8974,7 +8966,7 @@
     </row>
     <row r="99" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C99" s="121" t="s">
@@ -9057,10 +9049,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="195"/>
+      <c r="B1" s="198"/>
       <c r="D1" s="185" t="s">
         <v>57</v>
       </c>
@@ -9078,44 +9070,43 @@
         <v>42</v>
       </c>
       <c r="J1" s="75" t="e">
-        <f t="array" aca="1" ref="J1:J126" ca="1">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>#NAME?</v>
+        <f t="array" ref="J1:J126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="191" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="197">
-        <v>0</v>
-      </c>
-      <c r="D2" s="76" t="str">
+      <c r="B2" s="192">
+        <v>0</v>
+      </c>
+      <c r="D2" s="76" t="e">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_00328</v>
-      </c>
-      <c r="E2" s="76" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E2" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D2),"LastFixing","D"),"Libor","")</f>
-        <v>JpySND_Quote</v>
-      </c>
-      <c r="F2" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F2" s="77" t="e">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>4.2860000000000001E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G2" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
         <v>0</v>
       </c>
-      <c r="H2" s="86">
+      <c r="H2" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41948</v>
-      </c>
-      <c r="I2" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41949</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J2" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K2" s="78"/>
     </row>
@@ -9126,32 +9117,31 @@
       <c r="B3" s="80">
         <v>0</v>
       </c>
-      <c r="D3" s="76" t="str">
-        <v>obj_00322</v>
-      </c>
-      <c r="E3" s="76" t="str">
+      <c r="D3" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E3" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D3),"LastFixing","D"),"Libor","")</f>
-        <v>JpySWD_Quote</v>
-      </c>
-      <c r="F3" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" s="77" t="e">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>5.1429999999999998E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G3" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
         <v>0</v>
       </c>
-      <c r="H3" s="86">
+      <c r="H3" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41947</v>
-      </c>
-      <c r="I3" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41954</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J3" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K3" s="78"/>
     </row>
@@ -9162,32 +9152,31 @@
       <c r="B4" s="80">
         <v>2</v>
       </c>
-      <c r="D4" s="76" t="str">
-        <v>obj_0031d</v>
-      </c>
-      <c r="E4" s="76" t="str">
+      <c r="D4" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E4" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D4),"LastFixing","D"),"Libor","")</f>
-        <v>Jpy1MD_Quote</v>
-      </c>
-      <c r="F4" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" s="77" t="e">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>8.3000000000000001E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G4" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
         <v>0</v>
       </c>
-      <c r="H4" s="86">
+      <c r="H4" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41947</v>
-      </c>
-      <c r="I4" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41977</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J4" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K4" s="78"/>
     </row>
@@ -9198,577 +9187,558 @@
       <c r="B5" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="76" t="str">
-        <v>obj_00320</v>
-      </c>
-      <c r="E5" s="76" t="str">
+      <c r="D5" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E5" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D5),"LastFixing","D"),"Libor","")</f>
-        <v>Jpy2MD_Quote</v>
-      </c>
-      <c r="F5" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F5" s="77" t="e">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>9.9290000000000012E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G5" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
         <v>0</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41947</v>
-      </c>
-      <c r="I5" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I5" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42009</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J5" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K5" s="78"/>
     </row>
     <row r="6" spans="1:11" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="198" t="s">
+      <c r="A6" s="193" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="82" t="str">
-        <f>_xll.ohRangeRetrieveError(Selected!D2)</f>
-        <v/>
-      </c>
-      <c r="D6" s="76" t="str">
-        <v>obj_00323</v>
-      </c>
-      <c r="E6" s="76" t="str">
+        <f ca="1">_xll.ohRangeRetrieveError(Selected!D2)</f>
+        <v>qlRateHelperSelection - ObjectHandler error: attempt to retrieve object with unknown ID 'obj_00322'</v>
+      </c>
+      <c r="D6" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E6" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D6),"LastFixing","D"),"Libor","")</f>
-        <v>Jpy3MD_Quote</v>
-      </c>
-      <c r="F6" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F6" s="77" t="e">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>1.1357000000000001E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G6" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="86">
+      <c r="H6" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41947</v>
-      </c>
-      <c r="I6" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>42039</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J6" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K6" s="78"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D7" s="76" t="str">
-        <v>obj_00316</v>
-      </c>
-      <c r="E7" s="76" t="str">
+      <c r="D7" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E7" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D7),"LastFixing","D"),"Libor","")</f>
-        <v>Jpy6MD_Quote</v>
-      </c>
-      <c r="F7" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F7" s="77" t="e">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1.6142999999999999E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G7" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="86">
+      <c r="H7" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41947</v>
-      </c>
-      <c r="I7" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I7" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>42129</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J7" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K7" s="78"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D8" s="76" t="str">
-        <v>obj_00326</v>
-      </c>
-      <c r="E8" s="76" t="str">
+      <c r="D8" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E8" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D8),"LastFixing","D"),"Libor","")</f>
-        <v>Jpy1YD_Quote</v>
-      </c>
-      <c r="F8" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F8" s="77" t="e">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>3.0042999999999997E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G8" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="86">
+      <c r="H8" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41947</v>
-      </c>
-      <c r="I8" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I8" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42312</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J8" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K8" s="78"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D9" s="76" t="str">
-        <v>obj_00329</v>
-      </c>
-      <c r="E9" s="76" t="str">
+      <c r="D9" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E9" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D9),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L1Y_Quote</v>
-      </c>
-      <c r="F9" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F9" s="77" t="e">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>1.575E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G9" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
         <v>0</v>
       </c>
-      <c r="H9" s="86">
+      <c r="H9" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41948</v>
-      </c>
-      <c r="I9" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I9" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42313</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J9" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K9" s="78"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D10" s="76" t="str">
-        <v>obj_00348</v>
-      </c>
-      <c r="E10" s="76" t="str">
+      <c r="D10" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E10" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D10),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L18M_Quote</v>
-      </c>
-      <c r="F10" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F10" s="77" t="e">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>1.5499999999999999E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G10" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
         <v>0</v>
       </c>
-      <c r="H10" s="86">
+      <c r="H10" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41948</v>
-      </c>
-      <c r="I10" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I10" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42496</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J10" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K10" s="78"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D11" s="76" t="str">
-        <v>obj_0033e</v>
-      </c>
-      <c r="E11" s="76" t="str">
+      <c r="D11" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E11" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D11),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L3Y_Quote</v>
-      </c>
-      <c r="F11" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" s="77" t="e">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>1.65E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G11" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
         <v>0</v>
       </c>
-      <c r="H11" s="86">
+      <c r="H11" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41948</v>
-      </c>
-      <c r="I11" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>43045</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J11" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K11" s="78"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D12" s="76" t="str">
-        <v>obj_0032e</v>
-      </c>
-      <c r="E12" s="76" t="str">
+      <c r="D12" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E12" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D12),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L4Y_Quote</v>
-      </c>
-      <c r="F12" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F12" s="77" t="e">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>1.9250000000000001E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G12" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
         <v>0</v>
       </c>
-      <c r="H12" s="86">
+      <c r="H12" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41948</v>
-      </c>
-      <c r="I12" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I12" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>43409</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J12" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K12" s="78"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D13" s="76" t="str">
-        <v>obj_0035e</v>
-      </c>
-      <c r="E13" s="76" t="str">
+      <c r="D13" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E13" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D13),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L5Y_Quote</v>
-      </c>
-      <c r="F13" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="77" t="e">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>2.3749999999999999E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G13" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
         <v>0</v>
       </c>
-      <c r="H13" s="86">
+      <c r="H13" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41948</v>
-      </c>
-      <c r="I13" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I13" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>43774</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J13" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K13" s="78"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D14" s="76" t="str">
-        <v>obj_00344</v>
-      </c>
-      <c r="E14" s="76" t="str">
+      <c r="D14" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E14" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D14),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L6Y_Quote</v>
-      </c>
-      <c r="F14" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="77" t="e">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>2.9749999999999998E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G14" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
         <v>0</v>
       </c>
-      <c r="H14" s="86">
+      <c r="H14" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41948</v>
-      </c>
-      <c r="I14" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I14" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>44140</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J14" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K14" s="78"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D15" s="76" t="str">
-        <v>obj_0036a</v>
-      </c>
-      <c r="E15" s="76" t="str">
+      <c r="D15" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E15" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D15),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L7Y_Quote</v>
-      </c>
-      <c r="F15" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" s="77" t="e">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>3.6750000000000003E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G15" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
         <v>0</v>
       </c>
-      <c r="H15" s="86">
+      <c r="H15" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41948</v>
-      </c>
-      <c r="I15" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I15" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>44505</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J15" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K15" s="78"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="76" t="str">
-        <v>obj_00369</v>
-      </c>
-      <c r="E16" s="76" t="str">
+      <c r="D16" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E16" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D16),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L8Y_Quote</v>
-      </c>
-      <c r="F16" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F16" s="77" t="e">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>4.3999999999999994E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G16" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
         <v>0</v>
       </c>
-      <c r="H16" s="86">
+      <c r="H16" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41948</v>
-      </c>
-      <c r="I16" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>44872</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J16" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D17" s="76" t="str">
-        <v>obj_0034b</v>
-      </c>
-      <c r="E17" s="76" t="str">
+      <c r="D17" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E17" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D17),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L9Y_Quote</v>
-      </c>
-      <c r="F17" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" s="77" t="e">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>5.1749999999999999E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G17" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
         <v>0</v>
       </c>
-      <c r="H17" s="86">
+      <c r="H17" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41948</v>
-      </c>
-      <c r="I17" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I17" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>45236</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J17" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D18" s="76" t="str">
-        <v>obj_00357</v>
-      </c>
-      <c r="E18" s="76" t="str">
+      <c r="D18" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E18" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D18),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L10Y_Quote</v>
-      </c>
-      <c r="F18" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="77" t="e">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>5.9250000000000006E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G18" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
         <v>0</v>
       </c>
-      <c r="H18" s="86">
+      <c r="H18" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41948</v>
-      </c>
-      <c r="I18" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>45601</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J18" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D19" s="76" t="str">
-        <v>obj_00346</v>
-      </c>
-      <c r="E19" s="76" t="str">
+      <c r="D19" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E19" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D19),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L12Y_Quote</v>
-      </c>
-      <c r="F19" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="77" t="e">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>7.5500000000000003E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G19" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
         <v>0</v>
       </c>
-      <c r="H19" s="86">
+      <c r="H19" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41948</v>
-      </c>
-      <c r="I19" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>46331</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J19" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D20" s="76" t="str">
-        <v>obj_00354</v>
-      </c>
-      <c r="E20" s="76" t="str">
+      <c r="D20" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E20" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D20),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L15Y_Quote</v>
-      </c>
-      <c r="F20" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="77" t="e">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>9.9750000000000012E-3</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G20" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
         <v>0</v>
       </c>
-      <c r="H20" s="86">
+      <c r="H20" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41948</v>
-      </c>
-      <c r="I20" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>47427</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J20" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D21" s="76" t="str">
-        <v>obj_00361</v>
-      </c>
-      <c r="E21" s="76" t="str">
+      <c r="D21" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E21" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D21),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L20Y_Quote</v>
-      </c>
-      <c r="F21" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F21" s="77" t="e">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>1.3025E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G21" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
         <v>0</v>
       </c>
-      <c r="H21" s="86">
+      <c r="H21" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41948</v>
-      </c>
-      <c r="I21" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I21" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>49254</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J21" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="76" t="str">
-        <v>obj_0036f</v>
-      </c>
-      <c r="E22" s="76" t="str">
+      <c r="D22" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E22" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D22),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L25Y_Quote</v>
-      </c>
-      <c r="F22" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F22" s="77" t="e">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.4649999999999998E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G22" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
         <v>0</v>
       </c>
-      <c r="H22" s="86">
+      <c r="H22" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41948</v>
-      </c>
-      <c r="I22" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I22" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>51081</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J22" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D23" s="76" t="str">
-        <v>obj_00377</v>
-      </c>
-      <c r="E23" s="76" t="str">
+      <c r="D23" s="76" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="E23" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D23),"LastFixing","D"),"Libor","")</f>
-        <v>JPYSB6L30Y_Quote</v>
-      </c>
-      <c r="F23" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F23" s="77" t="e">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.55E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G23" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
         <v>0</v>
       </c>
-      <c r="H23" s="86">
+      <c r="H23" s="86" t="e">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41948</v>
-      </c>
-      <c r="I23" s="87">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" s="87" t="e">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>52908</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J23" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D24" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E24" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D24),"LastFixing","D"),"Libor","")</f>
@@ -9791,13 +9761,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J24" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D25" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E25" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D25),"LastFixing","D"),"Libor","")</f>
@@ -9820,13 +9789,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J25" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D26" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E26" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D26),"LastFixing","D"),"Libor","")</f>
@@ -9849,13 +9817,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J26" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D27" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E27" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D27),"LastFixing","D"),"Libor","")</f>
@@ -9878,13 +9845,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J27" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D28" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E28" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D28),"LastFixing","D"),"Libor","")</f>
@@ -9907,13 +9873,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J28" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D29" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E29" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D29),"LastFixing","D"),"Libor","")</f>
@@ -9936,13 +9901,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J29" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D30" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E30" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D30),"LastFixing","D"),"Libor","")</f>
@@ -9965,13 +9929,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J30" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D31" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E31" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D31),"LastFixing","D"),"Libor","")</f>
@@ -9994,13 +9957,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J31" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D32" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E32" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D32),"LastFixing","D"),"Libor","")</f>
@@ -10023,13 +9985,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J32" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D33" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E33" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D33),"LastFixing","D"),"Libor","")</f>
@@ -10052,13 +10013,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J33" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D34" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E34" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D34),"LastFixing","D"),"Libor","")</f>
@@ -10081,13 +10041,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J34" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D35" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E35" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D35),"LastFixing","D"),"Libor","")</f>
@@ -10110,13 +10069,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J35" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D36" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E36" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D36),"LastFixing","D"),"Libor","")</f>
@@ -10139,13 +10097,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J36" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D37" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E37" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D37),"LastFixing","D"),"Libor","")</f>
@@ -10168,13 +10125,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J37" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D38" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E38" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D38),"LastFixing","D"),"Libor","")</f>
@@ -10197,13 +10153,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J38" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D39" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E39" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D39),"LastFixing","D"),"Libor","")</f>
@@ -10226,13 +10181,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J39" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D40" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E40" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D40),"LastFixing","D"),"Libor","")</f>
@@ -10255,13 +10209,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J40" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D41" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E41" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D41),"LastFixing","D"),"Libor","")</f>
@@ -10284,13 +10237,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J41" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D42" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E42" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D42),"LastFixing","D"),"Libor","")</f>
@@ -10313,13 +10265,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J42" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D43" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E43" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D43),"LastFixing","D"),"Libor","")</f>
@@ -10342,13 +10293,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J43" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D44" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E44" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D44),"LastFixing","D"),"Libor","")</f>
@@ -10371,13 +10321,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J44" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D45" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E45" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D45),"LastFixing","D"),"Libor","")</f>
@@ -10400,13 +10349,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J45" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D46" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E46" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D46),"LastFixing","D"),"Libor","")</f>
@@ -10429,13 +10377,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J46" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D47" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E47" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D47),"LastFixing","D"),"Libor","")</f>
@@ -10458,13 +10405,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J47" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="48" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D48" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E48" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D48),"LastFixing","D"),"Libor","")</f>
@@ -10487,13 +10433,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J48" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D49" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E49" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D49),"LastFixing","D"),"Libor","")</f>
@@ -10516,13 +10461,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J49" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D50" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E50" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D50),"LastFixing","D"),"Libor","")</f>
@@ -10545,13 +10489,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J50" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D51" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E51" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D51),"LastFixing","D"),"Libor","")</f>
@@ -10574,13 +10517,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J51" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D52" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E52" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D52),"LastFixing","D"),"Libor","")</f>
@@ -10603,13 +10545,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J52" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="53" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D53" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E53" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D53),"LastFixing","D"),"Libor","")</f>
@@ -10632,13 +10573,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J53" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D54" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E54" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D54),"LastFixing","D"),"Libor","")</f>
@@ -10661,13 +10601,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J54" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D55" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E55" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D55),"LastFixing","D"),"Libor","")</f>
@@ -10690,13 +10629,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J55" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D56" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E56" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D56),"LastFixing","D"),"Libor","")</f>
@@ -10719,13 +10657,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J56" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="57" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D57" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E57" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D57),"LastFixing","D"),"Libor","")</f>
@@ -10748,13 +10685,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J57" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D58" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E58" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D58),"LastFixing","D"),"Libor","")</f>
@@ -10777,13 +10713,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J58" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D59" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E59" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D59),"LastFixing","D"),"Libor","")</f>
@@ -10806,13 +10741,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J59" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D60" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E60" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D60),"LastFixing","D"),"Libor","")</f>
@@ -10835,13 +10769,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J60" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D61" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E61" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D61),"LastFixing","D"),"Libor","")</f>
@@ -10864,13 +10797,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J61" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D62" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E62" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D62),"LastFixing","D"),"Libor","")</f>
@@ -10893,13 +10825,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J62" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D63" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E63" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D63),"LastFixing","D"),"Libor","")</f>
@@ -10922,13 +10853,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J63" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="64" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D64" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E64" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D64),"LastFixing","D"),"Libor","")</f>
@@ -10951,13 +10881,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J64" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="65" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D65" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E65" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D65),"LastFixing","D"),"Libor","")</f>
@@ -10980,13 +10909,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J65" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="66" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D66" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E66" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D66),"LastFixing","D"),"Libor","")</f>
@@ -11009,13 +10937,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J66" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="67" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D67" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E67" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D67),"LastFixing","D"),"Libor","")</f>
@@ -11038,13 +10965,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J67" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="68" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D68" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E68" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D68),"LastFixing","D"),"Libor","")</f>
@@ -11067,13 +10993,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J68" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="69" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D69" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E69" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D69),"LastFixing","D"),"Libor","")</f>
@@ -11096,13 +11021,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J69" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="70" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D70" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E70" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D70),"LastFixing","D"),"Libor","")</f>
@@ -11125,13 +11049,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J70" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D71" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E71" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D71),"LastFixing","D"),"Libor","")</f>
@@ -11154,13 +11077,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J71" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D72" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E72" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D72),"LastFixing","D"),"Libor","")</f>
@@ -11183,13 +11105,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J72" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="73" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D73" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E73" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D73),"LastFixing","D"),"Libor","")</f>
@@ -11212,13 +11133,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J73" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="74" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D74" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E74" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D74),"LastFixing","D"),"Libor","")</f>
@@ -11241,13 +11161,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J74" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="75" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D75" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E75" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D75),"LastFixing","D"),"Libor","")</f>
@@ -11270,13 +11189,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J75" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="76" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D76" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E76" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D76),"LastFixing","D"),"Libor","")</f>
@@ -11299,13 +11217,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J76" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="77" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D77" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E77" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D77),"LastFixing","D"),"Libor","")</f>
@@ -11328,13 +11245,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J77" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="78" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D78" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E78" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D78),"LastFixing","D"),"Libor","")</f>
@@ -11357,13 +11273,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J78" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="79" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D79" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E79" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D79),"LastFixing","D"),"Libor","")</f>
@@ -11386,13 +11301,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J79" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="80" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D80" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E80" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D80),"LastFixing","D"),"Libor","")</f>
@@ -11415,13 +11329,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J80" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="81" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D81" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E81" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D81),"LastFixing","D"),"Libor","")</f>
@@ -11444,13 +11357,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J81" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="82" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D82" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E82" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D82),"LastFixing","D"),"Libor","")</f>
@@ -11473,13 +11385,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J82" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="83" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D83" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E83" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D83),"LastFixing","D"),"Libor","")</f>
@@ -11502,13 +11413,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J83" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="84" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D84" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E84" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D84),"LastFixing","D"),"Libor","")</f>
@@ -11531,13 +11441,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J84" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="85" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D85" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E85" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D85),"LastFixing","D"),"Libor","")</f>
@@ -11560,13 +11469,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J85" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="86" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D86" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E86" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D86),"LastFixing","D"),"Libor","")</f>
@@ -11589,13 +11497,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J86" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="87" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D87" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E87" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D87),"LastFixing","D"),"Libor","")</f>
@@ -11618,13 +11525,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J87" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="88" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D88" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E88" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D88),"LastFixing","D"),"Libor","")</f>
@@ -11647,13 +11553,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J88" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="89" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D89" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E89" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D89),"LastFixing","D"),"Libor","")</f>
@@ -11676,13 +11581,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J89" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="90" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D90" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E90" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D90),"LastFixing","D"),"Libor","")</f>
@@ -11705,13 +11609,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J90" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="91" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D91" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E91" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D91),"LastFixing","D"),"Libor","")</f>
@@ -11734,13 +11637,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J91" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="92" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D92" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E92" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D92),"LastFixing","D"),"Libor","")</f>
@@ -11763,13 +11665,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J92" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="93" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D93" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E93" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D93),"LastFixing","D"),"Libor","")</f>
@@ -11792,13 +11693,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J93" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="94" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D94" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E94" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D94),"LastFixing","D"),"Libor","")</f>
@@ -11821,13 +11721,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J94" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="95" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D95" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E95" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D95),"LastFixing","D"),"Libor","")</f>
@@ -11850,13 +11749,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J95" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="96" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D96" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E96" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D96),"LastFixing","D"),"Libor","")</f>
@@ -11879,13 +11777,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J96" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="97" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D97" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E97" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D97),"LastFixing","D"),"Libor","")</f>
@@ -11908,13 +11805,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J97" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="98" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D98" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E98" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D98),"LastFixing","D"),"Libor","")</f>
@@ -11937,13 +11833,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J98" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="99" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D99" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E99" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D99),"LastFixing","D"),"Libor","")</f>
@@ -11966,13 +11861,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J99" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="100" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D100" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E100" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D100),"LastFixing","D"),"Libor","")</f>
@@ -11995,13 +11889,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J100" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="101" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D101" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E101" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D101),"LastFixing","D"),"Libor","")</f>
@@ -12024,13 +11917,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J101" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="102" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D102" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E102" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D102),"LastFixing","D"),"Libor","")</f>
@@ -12053,13 +11945,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J102" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="103" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D103" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E103" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D103),"LastFixing","D"),"Libor","")</f>
@@ -12082,13 +11973,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J103" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="104" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D104" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E104" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D104),"LastFixing","D"),"Libor","")</f>
@@ -12111,13 +12001,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J104" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="105" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D105" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E105" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D105),"LastFixing","D"),"Libor","")</f>
@@ -12140,13 +12029,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J105" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="106" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D106" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E106" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D106),"LastFixing","D"),"Libor","")</f>
@@ -12169,13 +12057,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J106" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="107" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D107" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E107" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D107),"LastFixing","D"),"Libor","")</f>
@@ -12198,13 +12085,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J107" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="108" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D108" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E108" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D108),"LastFixing","D"),"Libor","")</f>
@@ -12227,13 +12113,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J108" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="109" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D109" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E109" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D109),"LastFixing","D"),"Libor","")</f>
@@ -12256,13 +12141,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J109" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="110" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D110" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E110" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D110),"LastFixing","D"),"Libor","")</f>
@@ -12285,13 +12169,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J110" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="111" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D111" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E111" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D111),"LastFixing","D"),"Libor","")</f>
@@ -12314,13 +12197,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J111" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="112" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D112" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E112" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D112),"LastFixing","D"),"Libor","")</f>
@@ -12343,13 +12225,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J112" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="113" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D113" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E113" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D113),"LastFixing","D"),"Libor","")</f>
@@ -12372,13 +12253,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J113" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="114" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D114" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E114" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D114),"LastFixing","D"),"Libor","")</f>
@@ -12401,13 +12281,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J114" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="115" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D115" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E115" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D115),"LastFixing","D"),"Libor","")</f>
@@ -12430,13 +12309,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J115" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="116" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D116" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E116" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D116),"LastFixing","D"),"Libor","")</f>
@@ -12459,13 +12337,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J116" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="117" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D117" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E117" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D117),"LastFixing","D"),"Libor","")</f>
@@ -12488,13 +12365,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J117" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="118" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D118" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E118" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D118),"LastFixing","D"),"Libor","")</f>
@@ -12517,13 +12393,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J118" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="119" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D119" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E119" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D119),"LastFixing","D"),"Libor","")</f>
@@ -12546,13 +12421,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J119" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="120" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D120" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E120" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D120),"LastFixing","D"),"Libor","")</f>
@@ -12575,13 +12449,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J120" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="121" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D121" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E121" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D121),"LastFixing","D"),"Libor","")</f>
@@ -12604,13 +12477,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J121" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="122" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D122" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E122" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D122),"LastFixing","D"),"Libor","")</f>
@@ -12633,13 +12505,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J122" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="123" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D123" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E123" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D123),"LastFixing","D"),"Libor","")</f>
@@ -12662,13 +12533,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J123" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="124" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D124" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E124" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D124),"LastFixing","D"),"Libor","")</f>
@@ -12691,13 +12561,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J124" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="125" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D125" s="76" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E125" s="76" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D125),"LastFixing","D"),"Libor","")</f>
@@ -12720,13 +12589,12 @@
         <v>#VALUE!</v>
       </c>
       <c r="J125" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="126" spans="4:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D126" s="83" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="E126" s="83" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D126),"LastFixing","D"),"Libor","")</f>
@@ -12749,8 +12617,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J126" s="75" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>